<commit_message>
Added even more to MasterCollection.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/ShaneAndShane/Shane & Shane (from website) V2.xlsx
+++ b/WorshipCreator.TestData/Source/Books/ShaneAndShane/Shane & Shane (from website) V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\ShaneAndShane\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C50E284-3122-4B8E-B5AD-AB30AAFC7B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E3B5F9-C8F3-4116-A9BB-CF1F4D373744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1898BBCD-4A5D-4B3F-9317-061045B18130}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="771">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="763">
   <si>
     <t>G</t>
   </si>
@@ -2317,40 +2317,16 @@
     <t>Psalms 2</t>
   </si>
   <si>
-    <t>Battle Belongs</t>
-  </si>
-  <si>
-    <t>At Your Name (Lite)</t>
-  </si>
-  <si>
-    <t>Raise A Hallelujah (Lite)</t>
-  </si>
-  <si>
-    <t>Peace (Lite)</t>
-  </si>
-  <si>
-    <t>Bigger Than I Thought (Lite)</t>
-  </si>
-  <si>
-    <t>Sinking Deep (Lite)</t>
-  </si>
-  <si>
-    <t>Psalm 145 (Lite)</t>
-  </si>
-  <si>
-    <t>Psalm 13 (Lite)</t>
-  </si>
-  <si>
-    <t>The One You'll Find (Lite)</t>
-  </si>
-  <si>
-    <t>Great Reward (Lite)</t>
-  </si>
-  <si>
     <t>WI Lite</t>
   </si>
   <si>
     <t>Lite</t>
+  </si>
+  <si>
+    <t>Singles</t>
+  </si>
+  <si>
+    <t>WI Singles</t>
   </si>
 </sst>
 </file>
@@ -2419,7 +2395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2443,6 +2419,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2963,12 +2942,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B95710C-65C8-40EA-B639-B1B45687620A}">
-  <dimension ref="A1:W313"/>
+  <dimension ref="A1:W314"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="K313" sqref="K313"/>
+      <selection pane="bottomLeft" activeCell="G314" sqref="G314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17405,16 +17384,16 @@
     </row>
     <row r="304" spans="1:12">
       <c r="A304" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B304">
         <v>1</v>
       </c>
       <c r="C304" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D304" t="s">
-        <v>759</v>
+        <v>330</v>
       </c>
       <c r="E304" t="str">
         <f t="shared" si="40"/>
@@ -17430,7 +17409,13 @@
       </c>
       <c r="H304" t="str">
         <f t="shared" si="43"/>
-        <v/>
+        <v>Phil Wickham</v>
+      </c>
+      <c r="I304">
+        <v>81</v>
+      </c>
+      <c r="J304" t="s">
+        <v>147</v>
       </c>
       <c r="K304" s="3">
         <v>7148126</v>
@@ -17438,16 +17423,16 @@
     </row>
     <row r="305" spans="1:11">
       <c r="A305" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B305">
         <v>2</v>
       </c>
       <c r="C305" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D305" t="s">
-        <v>760</v>
+        <v>331</v>
       </c>
       <c r="E305" t="str">
         <f t="shared" si="40"/>
@@ -17463,7 +17448,13 @@
       </c>
       <c r="H305" t="str">
         <f t="shared" si="43"/>
-        <v/>
+        <v>Phil Wickham</v>
+      </c>
+      <c r="I305">
+        <v>84</v>
+      </c>
+      <c r="J305" t="s">
+        <v>24</v>
       </c>
       <c r="K305" s="3">
         <v>5942543</v>
@@ -17471,23 +17462,23 @@
     </row>
     <row r="306" spans="1:11">
       <c r="A306" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B306">
         <v>3</v>
       </c>
       <c r="C306" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D306" t="s">
-        <v>761</v>
+        <v>335</v>
       </c>
       <c r="E306" t="str">
-        <f t="shared" ref="E306:E313" si="44">IF(ISNUMBER(SEARCH(" by", D306)), LEFT(D306, FIND(" by ",D306) - 1),D306)</f>
+        <f t="shared" ref="E306:E314" si="44">IF(ISNUMBER(SEARCH(" by", D306)), LEFT(D306, FIND(" by ",D306) - 1),D306)</f>
         <v>Raise A Hallelujah (Lite)</v>
       </c>
       <c r="F306" t="str">
-        <f t="shared" ref="F306:F313" si="45">LEFT(E306,IF(ISNUMBER(SEARCH(" (",E306)),FIND(" (",E306)-1,LEN(E306)))</f>
+        <f t="shared" ref="F306:F314" si="45">LEFT(E306,IF(ISNUMBER(SEARCH(" (",E306)),FIND(" (",E306)-1,LEN(E306)))</f>
         <v>Raise A Hallelujah</v>
       </c>
       <c r="G306" t="str">
@@ -17496,7 +17487,13 @@
       </c>
       <c r="H306" t="str">
         <f t="shared" ref="H306:H313" si="47">IF(ISNUMBER(SEARCH(" by",D306)),RIGHT(D306, LEN(D306) - FIND(" by ",D306) - 3),"")</f>
-        <v/>
+        <v>Jonathan David &amp; Melissa Helser</v>
+      </c>
+      <c r="I306">
+        <v>82</v>
+      </c>
+      <c r="J306" t="s">
+        <v>3</v>
       </c>
       <c r="K306" s="3">
         <v>7119315</v>
@@ -17504,16 +17501,16 @@
     </row>
     <row r="307" spans="1:11">
       <c r="A307" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B307">
         <v>4</v>
       </c>
       <c r="C307" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D307" t="s">
-        <v>762</v>
+        <v>338</v>
       </c>
       <c r="E307" t="str">
         <f t="shared" si="44"/>
@@ -17529,7 +17526,13 @@
       </c>
       <c r="H307" t="str">
         <f t="shared" si="47"/>
-        <v/>
+        <v>Hillsong Young &amp; Free</v>
+      </c>
+      <c r="I307">
+        <v>64</v>
+      </c>
+      <c r="J307" t="s">
+        <v>29</v>
       </c>
       <c r="K307" s="3">
         <v>7104628</v>
@@ -17537,16 +17540,16 @@
     </row>
     <row r="308" spans="1:11">
       <c r="A308" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B308">
         <v>5</v>
       </c>
       <c r="C308" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D308" t="s">
-        <v>763</v>
+        <v>339</v>
       </c>
       <c r="E308" t="str">
         <f t="shared" si="44"/>
@@ -17562,7 +17565,13 @@
       </c>
       <c r="H308" t="str">
         <f t="shared" si="47"/>
-        <v/>
+        <v>Passion</v>
+      </c>
+      <c r="I308">
+        <v>63</v>
+      </c>
+      <c r="J308" t="s">
+        <v>27</v>
       </c>
       <c r="K308" s="3">
         <v>7123203</v>
@@ -17570,16 +17579,16 @@
     </row>
     <row r="309" spans="1:11">
       <c r="A309" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B309">
         <v>6</v>
       </c>
       <c r="C309" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D309" t="s">
-        <v>764</v>
+        <v>337</v>
       </c>
       <c r="E309" t="str">
         <f t="shared" si="44"/>
@@ -17595,7 +17604,13 @@
       </c>
       <c r="H309" t="str">
         <f t="shared" si="47"/>
-        <v/>
+        <v>Hillsong Young &amp; Free</v>
+      </c>
+      <c r="I309">
+        <v>70</v>
+      </c>
+      <c r="J309" t="s">
+        <v>24</v>
       </c>
       <c r="K309" s="3">
         <v>6605236</v>
@@ -17603,16 +17618,16 @@
     </row>
     <row r="310" spans="1:11">
       <c r="A310" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B310">
         <v>7</v>
       </c>
       <c r="C310" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D310" t="s">
-        <v>765</v>
+        <v>333</v>
       </c>
       <c r="E310" t="str">
         <f t="shared" si="44"/>
@@ -17628,7 +17643,13 @@
       </c>
       <c r="H310" t="str">
         <f t="shared" si="47"/>
-        <v/>
+        <v>Shane &amp; Shane</v>
+      </c>
+      <c r="I310">
+        <v>80</v>
+      </c>
+      <c r="J310" t="s">
+        <v>0</v>
       </c>
       <c r="K310" s="3">
         <v>3407011</v>
@@ -17636,16 +17657,16 @@
     </row>
     <row r="311" spans="1:11">
       <c r="A311" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B311">
         <v>8</v>
       </c>
       <c r="C311" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D311" t="s">
-        <v>766</v>
+        <v>334</v>
       </c>
       <c r="E311" t="str">
         <f t="shared" si="44"/>
@@ -17661,7 +17682,13 @@
       </c>
       <c r="H311" t="str">
         <f t="shared" si="47"/>
-        <v/>
+        <v>Shane &amp; Shane</v>
+      </c>
+      <c r="I311">
+        <v>80</v>
+      </c>
+      <c r="J311" t="s">
+        <v>29</v>
       </c>
       <c r="K311" s="3">
         <v>3406988</v>
@@ -17669,16 +17696,16 @@
     </row>
     <row r="312" spans="1:11">
       <c r="A312" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B312">
         <v>9</v>
       </c>
       <c r="C312" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D312" t="s">
-        <v>767</v>
+        <v>332</v>
       </c>
       <c r="E312" t="str">
         <f t="shared" si="44"/>
@@ -17694,7 +17721,13 @@
       </c>
       <c r="H312" t="str">
         <f t="shared" si="47"/>
-        <v/>
+        <v>Shane &amp; Shane</v>
+      </c>
+      <c r="I312">
+        <v>118</v>
+      </c>
+      <c r="J312" t="s">
+        <v>29</v>
       </c>
       <c r="K312" s="3">
         <v>6590815</v>
@@ -17702,16 +17735,16 @@
     </row>
     <row r="313" spans="1:11">
       <c r="A313" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="B313">
         <v>10</v>
       </c>
       <c r="C313" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="D313" t="s">
-        <v>768</v>
+        <v>336</v>
       </c>
       <c r="E313" t="str">
         <f t="shared" si="44"/>
@@ -17727,10 +17760,55 @@
       </c>
       <c r="H313" t="str">
         <f t="shared" si="47"/>
-        <v/>
+        <v>Shane &amp; Shane</v>
+      </c>
+      <c r="I313">
+        <v>72</v>
+      </c>
+      <c r="J313" t="s">
+        <v>6</v>
       </c>
       <c r="K313" s="3">
         <v>5627789</v>
+      </c>
+    </row>
+    <row r="314" spans="1:11">
+      <c r="A314" t="s">
+        <v>761</v>
+      </c>
+      <c r="B314">
+        <v>1</v>
+      </c>
+      <c r="C314" t="s">
+        <v>762</v>
+      </c>
+      <c r="D314" t="s">
+        <v>341</v>
+      </c>
+      <c r="E314" t="str">
+        <f t="shared" si="44"/>
+        <v>Run</v>
+      </c>
+      <c r="F314" t="str">
+        <f t="shared" si="45"/>
+        <v>Run</v>
+      </c>
+      <c r="G314" t="str">
+        <f t="shared" ref="G314" si="48">IF(ISNUMBER(SEARCH("(",E314)), LEFT(RIGHT(E314, LEN(E314) - FIND("(",E314)), LEN(RIGHT(E314, LEN(E314) - FIND("(",E314))) - 1), "")</f>
+        <v/>
+      </c>
+      <c r="H314" t="str">
+        <f t="shared" ref="H314" si="49">IF(ISNUMBER(SEARCH(" by",D314)),RIGHT(D314, LEN(D314) - FIND(" by ",D314) - 3),"")</f>
+        <v>Liberty Worship Collective</v>
+      </c>
+      <c r="I314">
+        <v>85</v>
+      </c>
+      <c r="J314" t="s">
+        <v>6</v>
+      </c>
+      <c r="K314" s="11">
+        <v>7087777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>